<commit_message>
Add more work log functions
</commit_message>
<xml_diff>
--- a/Varpas 1.xlsx
+++ b/Varpas 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="37">
   <si>
     <t/>
   </si>
@@ -121,10 +121,10 @@
     <t>0</t>
   </si>
   <si>
+    <t>Jauns efwefew</t>
+  </si>
+  <si>
     <t>Signe Zalužinska</t>
-  </si>
-  <si>
-    <t>fwefwf wfwefwe</t>
   </si>
 </sst>
 </file>
@@ -750,7 +750,7 @@
         <v>34</v>
       </c>
       <c r="K3">
-        <v>-431911</v>
+        <v>0</v>
       </c>
       <c r="L3" t="s">
         <v>34</v>
@@ -813,10 +813,10 @@
         <v>34</v>
       </c>
       <c r="AF3">
-        <v>-431911</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>-17996.291666666668</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -847,11 +847,11 @@
       <c r="I4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="J4" t="s">
+        <v>34</v>
       </c>
       <c r="K4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L4" t="s">
         <v>34</v>
@@ -914,10 +914,10 @@
         <v>34</v>
       </c>
       <c r="AF4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AG4">
-        <v>0.2916666666666667</v>
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more export functionality
</commit_message>
<xml_diff>
--- a/Varpas 1.xlsx
+++ b/Varpas 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t/>
   </si>
@@ -109,6 +109,9 @@
     <t>30</t>
   </si>
   <si>
+    <t>31</t>
+  </si>
+  <si>
     <t>Kopā</t>
   </si>
   <si>
@@ -118,25 +121,7 @@
     <t>Nils Asejevs</t>
   </si>
   <si>
-    <t>25.00</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>27.00</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>Signe Zalužinska</t>
-  </si>
-  <si>
-    <t>9.00</t>
-  </si>
-  <si>
-    <t>Jauns efwefew</t>
   </si>
 </sst>
 </file>
@@ -520,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AH3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="31" width="5" customWidth="1"/>
-    <col min="32" max="33" width="10" customWidth="1"/>
+    <col min="2" max="32" width="5" customWidth="1"/>
+    <col min="33" max="34" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,13 +529,13 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -565,13 +550,13 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
       <c r="P1" t="s">
@@ -586,13 +571,13 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
@@ -607,13 +592,13 @@
       <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
       <c r="AD1" t="s">
@@ -628,10 +613,13 @@
       <c r="AG1" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -640,100 +628,103 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>26</v>
+      </c>
+      <c r="AH2">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>54</v>
-      </c>
-      <c r="AG2">
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
       <c r="B3">
         <v>0</v>
       </c>
@@ -746,13 +737,13 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
@@ -761,19 +752,19 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
         <v>0</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
@@ -788,13 +779,13 @@
       <c r="S3">
         <v>0</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="1">
         <v>0</v>
       </c>
       <c r="U3" s="1">
         <v>0</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3">
         <v>0</v>
       </c>
       <c r="W3">
@@ -809,13 +800,13 @@
       <c r="Z3">
         <v>0</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="1">
         <v>0</v>
       </c>
       <c r="AB3" s="1">
         <v>0</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3">
@@ -825,115 +816,17 @@
         <v>0</v>
       </c>
       <c r="AF3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1">
-        <v>0</v>
-      </c>
-      <c r="V4" s="1">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG1"/>
+  <autoFilter ref="A1:AH1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added expirty to comments
</commit_message>
<xml_diff>
--- a/Varpas 1.xlsx
+++ b/Varpas 1.xlsx
@@ -628,97 +628,97 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
       <c r="AF2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AG2">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="AH2">
-        <v>3.25</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
@@ -816,13 +816,13 @@
         <v>0</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AH3">
-        <v>0</v>
+        <v>1.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>